<commit_message>
updated the empty boxes in "New Table 3"
</commit_message>
<xml_diff>
--- a/Tables/Tables-updated.xlsx
+++ b/Tables/Tables-updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shumi\Desktop\RestoreNet-Publish\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E7A7A-65FB-41FD-A07F-7D5282D6425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D27E9A5-84D9-4107-9499-05736D0E4A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="185">
   <si>
     <t>Response variables</t>
   </si>
@@ -1111,7 +1111,7 @@
       <sheetName val="nichevalues"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
@@ -7291,7 +7291,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="J17" sqref="J17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8039,8 +8039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BB0CE5-887D-4D47-90CD-EF50A904049A}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8192,14 +8192,14 @@
       <c r="D7" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="74" t="s">
-        <v>9</v>
+      <c r="E7" s="83">
+        <v>22.9416667421659</v>
+      </c>
+      <c r="F7" s="74">
+        <v>528</v>
+      </c>
+      <c r="G7" s="74">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -8293,14 +8293,14 @@
       <c r="D12" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="74" t="s">
-        <v>9</v>
+      <c r="E12" s="55">
+        <v>23.462500015894602</v>
+      </c>
+      <c r="F12" s="34">
+        <v>846</v>
+      </c>
+      <c r="G12" s="34">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -8359,14 +8359,14 @@
       <c r="D15" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="74" t="s">
-        <v>9</v>
+      <c r="E15" s="83">
+        <v>24.200000047683702</v>
+      </c>
+      <c r="F15" s="74">
+        <v>706</v>
+      </c>
+      <c r="G15" s="74">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -8425,14 +8425,14 @@
       <c r="D18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="74" t="s">
-        <v>9</v>
+      <c r="E18" s="83">
+        <v>23.412499964237199</v>
+      </c>
+      <c r="F18" s="74">
+        <v>423</v>
+      </c>
+      <c r="G18" s="74">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="29" x14ac:dyDescent="0.35">
@@ -9657,7 +9657,7 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>

</xml_diff>